<commit_message>
count "NS" (instead of ns) as non-apa
</commit_message>
<xml_diff>
--- a/inst/test_materials/manually_extracted_stats.xlsx
+++ b/inst/test_materials/manually_extracted_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnuijten\Documents\statcheck\inst\test_materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE55BE58-32FB-49B2-868F-226D93DF944D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FD507E-90B2-4B43-A611-CD5AE719A9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$AA$228</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AA$228</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2698" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2703" uniqueCount="319">
   <si>
     <t>journal</t>
   </si>
@@ -1002,6 +1002,9 @@
   </si>
   <si>
     <t>wrong spacing</t>
+  </si>
+  <si>
+    <t>capital ns is not strictly apa</t>
   </si>
 </sst>
 </file>
@@ -1397,9 +1400,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y2" sqref="Y2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA227" sqref="AA227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10381,7 +10384,7 @@
         <v>0.18</v>
       </c>
       <c r="X144">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y144">
         <v>0</v>
@@ -11102,7 +11105,7 @@
         <v>0</v>
       </c>
       <c r="Z155">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA155" t="s">
         <v>250</v>
@@ -12467,7 +12470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>295</v>
       </c>
@@ -12529,7 +12532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>295</v>
       </c>
@@ -12591,7 +12594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>295</v>
       </c>
@@ -12653,7 +12656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>295</v>
       </c>
@@ -12715,7 +12718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>295</v>
       </c>
@@ -12777,7 +12780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>295</v>
       </c>
@@ -12839,7 +12842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>295</v>
       </c>
@@ -12901,7 +12904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>295</v>
       </c>
@@ -12966,7 +12969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>295</v>
       </c>
@@ -13031,7 +13034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>295</v>
       </c>
@@ -13096,7 +13099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>295</v>
       </c>
@@ -13161,7 +13164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>295</v>
       </c>
@@ -13226,7 +13229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>295</v>
       </c>
@@ -13291,7 +13294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>295</v>
       </c>
@@ -13356,7 +13359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>295</v>
       </c>
@@ -13409,7 +13412,7 @@
         <v>182</v>
       </c>
       <c r="X191">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y191">
         <v>1</v>
@@ -13417,8 +13420,11 @@
       <c r="Z191">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA191" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="192" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>295</v>
       </c>
@@ -14505,7 +14511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>295</v>
       </c>
@@ -14567,7 +14573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>295</v>
       </c>
@@ -14617,7 +14623,7 @@
         <v>182</v>
       </c>
       <c r="X210">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y210">
         <v>1</v>
@@ -14625,8 +14631,11 @@
       <c r="Z210">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA210" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="211" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>295</v>
       </c>
@@ -14691,7 +14700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>295</v>
       </c>
@@ -14741,7 +14750,7 @@
         <v>182</v>
       </c>
       <c r="X212">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y212">
         <v>1</v>
@@ -14749,8 +14758,11 @@
       <c r="Z212">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA212" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="213" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>295</v>
       </c>
@@ -14812,7 +14824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>295</v>
       </c>
@@ -14874,7 +14886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>295</v>
       </c>
@@ -14936,7 +14948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>295</v>
       </c>
@@ -15001,7 +15013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>295</v>
       </c>
@@ -15066,7 +15078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>295</v>
       </c>
@@ -15131,7 +15143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>295</v>
       </c>
@@ -15193,7 +15205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>295</v>
       </c>
@@ -15255,7 +15267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>295</v>
       </c>
@@ -15317,7 +15329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>295</v>
       </c>
@@ -15367,7 +15379,7 @@
         <v>182</v>
       </c>
       <c r="X222">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y222">
         <v>1</v>
@@ -15375,8 +15387,11 @@
       <c r="Z222">
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA222" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="223" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>295</v>
       </c>
@@ -15438,7 +15453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>295</v>
       </c>
@@ -15500,7 +15515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>295</v>
       </c>
@@ -15562,7 +15577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>295</v>
       </c>
@@ -15624,7 +15639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>295</v>
       </c>
@@ -15674,7 +15689,7 @@
         <v>182</v>
       </c>
       <c r="X227">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y227">
         <v>1</v>
@@ -15682,8 +15697,11 @@
       <c r="Z227">
         <v>0</v>
       </c>
-    </row>
-    <row r="228" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA227" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="228" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>295</v>
       </c>
@@ -15746,11 +15764,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:AA228" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:AA228">
-      <sortCondition ref="C1:C190"/>
-    </sortState>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA228">
     <sortCondition ref="A1:A228"/>
   </sortState>

</xml_diff>

<commit_message>
classify a result as a typesetting issue
</commit_message>
<xml_diff>
--- a/inst/test_materials/manually_extracted_stats.xlsx
+++ b/inst/test_materials/manually_extracted_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnuijten\Documents\statcheck\inst\test_materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FD507E-90B2-4B43-A611-CD5AE719A9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3143264-A376-489A-84CA-31791D3E5FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2703" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2704" uniqueCount="320">
   <si>
     <t>journal</t>
   </si>
@@ -1005,6 +1005,9 @@
   </si>
   <si>
     <t>capital ns is not strictly apa</t>
+  </si>
+  <si>
+    <t>problem with rearranging columns: there is a lot of whitespace before the next column</t>
   </si>
 </sst>
 </file>
@@ -1400,9 +1403,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA227" sqref="AA227"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA132" sqref="AA132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9587,7 +9590,10 @@
         <v>0</v>
       </c>
       <c r="Z131">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AA131" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="132" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
count QT test as non apa
</commit_message>
<xml_diff>
--- a/inst/test_materials/manually_extracted_stats.xlsx
+++ b/inst/test_materials/manually_extracted_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnuijten\Documents\statcheck\inst\test_materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3143264-A376-489A-84CA-31791D3E5FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EAF777-7549-4202-8071-12D3EE4B7289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1404,8 +1404,8 @@
   <dimension ref="A1:AA228"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA132" sqref="AA132"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2285,7 +2285,7 @@
         <v>0.05</v>
       </c>
       <c r="X14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y14">
         <v>0</v>

</xml_diff>

<commit_message>
update: count NS (upper case) as apa
</commit_message>
<xml_diff>
--- a/inst/test_materials/manually_extracted_stats.xlsx
+++ b/inst/test_materials/manually_extracted_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnuijten\Documents\statcheck\inst\test_materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EAF777-7549-4202-8071-12D3EE4B7289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A48AA97-2A85-40B8-AB67-9B08D23B8D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2704" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2699" uniqueCount="319">
   <si>
     <t>journal</t>
   </si>
@@ -1002,9 +1002,6 @@
   </si>
   <si>
     <t>wrong spacing</t>
-  </si>
-  <si>
-    <t>capital ns is not strictly apa</t>
   </si>
   <si>
     <t>problem with rearranging columns: there is a lot of whitespace before the next column</t>
@@ -1403,9 +1400,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y14" sqref="Y14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y227" sqref="Y227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9593,7 +9590,7 @@
         <v>1</v>
       </c>
       <c r="AA131" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="132" spans="1:27" x14ac:dyDescent="0.25">
@@ -12476,7 +12473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>295</v>
       </c>
@@ -12538,7 +12535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>295</v>
       </c>
@@ -12600,7 +12597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>295</v>
       </c>
@@ -12662,7 +12659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>295</v>
       </c>
@@ -12724,7 +12721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>295</v>
       </c>
@@ -12786,7 +12783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>295</v>
       </c>
@@ -12848,7 +12845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>295</v>
       </c>
@@ -12910,7 +12907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>295</v>
       </c>
@@ -12975,7 +12972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>295</v>
       </c>
@@ -13040,7 +13037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>295</v>
       </c>
@@ -13105,7 +13102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>295</v>
       </c>
@@ -13170,7 +13167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>295</v>
       </c>
@@ -13235,7 +13232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>295</v>
       </c>
@@ -13300,7 +13297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>295</v>
       </c>
@@ -13365,7 +13362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>295</v>
       </c>
@@ -13418,7 +13415,7 @@
         <v>182</v>
       </c>
       <c r="X191">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y191">
         <v>1</v>
@@ -13426,11 +13423,8 @@
       <c r="Z191">
         <v>0</v>
       </c>
-      <c r="AA191" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="192" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="192" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>295</v>
       </c>
@@ -14517,7 +14511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>295</v>
       </c>
@@ -14579,7 +14573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>295</v>
       </c>
@@ -14629,7 +14623,7 @@
         <v>182</v>
       </c>
       <c r="X210">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y210">
         <v>1</v>
@@ -14637,11 +14631,8 @@
       <c r="Z210">
         <v>0</v>
       </c>
-      <c r="AA210" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="211" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="211" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>295</v>
       </c>
@@ -14706,7 +14697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>295</v>
       </c>
@@ -14756,7 +14747,7 @@
         <v>182</v>
       </c>
       <c r="X212">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y212">
         <v>1</v>
@@ -14764,11 +14755,8 @@
       <c r="Z212">
         <v>0</v>
       </c>
-      <c r="AA212" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="213" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>295</v>
       </c>
@@ -14830,7 +14818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>295</v>
       </c>
@@ -14892,7 +14880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>295</v>
       </c>
@@ -14954,7 +14942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>295</v>
       </c>
@@ -15019,7 +15007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>295</v>
       </c>
@@ -15084,7 +15072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>295</v>
       </c>
@@ -15149,7 +15137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>295</v>
       </c>
@@ -15211,7 +15199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>295</v>
       </c>
@@ -15273,7 +15261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>295</v>
       </c>
@@ -15335,7 +15323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>295</v>
       </c>
@@ -15385,7 +15373,7 @@
         <v>182</v>
       </c>
       <c r="X222">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y222">
         <v>1</v>
@@ -15393,11 +15381,8 @@
       <c r="Z222">
         <v>0</v>
       </c>
-      <c r="AA222" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="223" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="223" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>295</v>
       </c>
@@ -15459,7 +15444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>295</v>
       </c>
@@ -15521,7 +15506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>295</v>
       </c>
@@ -15583,7 +15568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>295</v>
       </c>
@@ -15645,7 +15630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>295</v>
       </c>
@@ -15695,7 +15680,7 @@
         <v>182</v>
       </c>
       <c r="X227">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y227">
         <v>1</v>
@@ -15703,11 +15688,8 @@
       <c r="Z227">
         <v>0</v>
       </c>
-      <c r="AA227" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="228" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="228" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>295</v>
       </c>

</xml_diff>